<commit_message>
new update after HQ's review
</commit_message>
<xml_diff>
--- a/output/2019/summary_sorted/summary_sorted_covid_analysis_2019_all_all.xlsx
+++ b/output/2019/summary_sorted/summary_sorted_covid_analysis_2019_all_all.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="395">
   <si>
     <t>governorate</t>
   </si>
@@ -137,40 +137,22 @@
     <t>c17_max</t>
   </si>
   <si>
-    <t>c18_i</t>
-  </si>
-  <si>
-    <t>c18_i_min</t>
-  </si>
-  <si>
-    <t>c18_i_max</t>
-  </si>
-  <si>
-    <t>c18_ii</t>
-  </si>
-  <si>
-    <t>c18_ii_min</t>
-  </si>
-  <si>
-    <t>c18_ii_max</t>
-  </si>
-  <si>
-    <t>c19_i</t>
-  </si>
-  <si>
-    <t>c19_i_min</t>
-  </si>
-  <si>
-    <t>c19_i_max</t>
-  </si>
-  <si>
-    <t>c19_ii</t>
-  </si>
-  <si>
-    <t>c19_ii_min</t>
-  </si>
-  <si>
-    <t>c19_ii_max</t>
+    <t>c18</t>
+  </si>
+  <si>
+    <t>c18_min</t>
+  </si>
+  <si>
+    <t>c18_max</t>
+  </si>
+  <si>
+    <t>c19</t>
+  </si>
+  <si>
+    <t>c19_min</t>
+  </si>
+  <si>
+    <t>c19_max</t>
   </si>
   <si>
     <t>c20</t>
@@ -353,6 +335,15 @@
     <t>c33_iii_max</t>
   </si>
   <si>
+    <t>c33_iv</t>
+  </si>
+  <si>
+    <t>c33_iv_min</t>
+  </si>
+  <si>
+    <t>c33_iv_max</t>
+  </si>
+  <si>
     <t>c37</t>
   </si>
   <si>
@@ -468,15 +459,6 @@
   </si>
   <si>
     <t>c47_iv_max</t>
-  </si>
-  <si>
-    <t>c48</t>
-  </si>
-  <si>
-    <t>c48_min</t>
-  </si>
-  <si>
-    <t>c48_max</t>
   </si>
   <si>
     <t>c49_i</t>
@@ -719,21 +701,6 @@
     <t>0.0362807730234022</t>
   </si>
   <si>
-    <t>Number of children with psychosocial distress (proxy data with behaviour change)</t>
-  </si>
-  <si>
-    <t>numerical</t>
-  </si>
-  <si>
-    <t>0.685533714525244</t>
-  </si>
-  <si>
-    <t>0.587069110175368</t>
-  </si>
-  <si>
-    <t>0.783998318875121</t>
-  </si>
-  <si>
     <t>% HH with adults with psychosocial distress (proxy data with behavior change)</t>
   </si>
   <si>
@@ -746,18 +713,6 @@
     <t>0.0534114660695324</t>
   </si>
   <si>
-    <t>Number of adults with psychosocial distress (proxy data with behavior change)</t>
-  </si>
-  <si>
-    <t>0.930081202944359</t>
-  </si>
-  <si>
-    <t>0.836969638367682</t>
-  </si>
-  <si>
-    <t>1.02319276752104</t>
-  </si>
-  <si>
     <t>% HHs with at least one person (adult OR child) with signs of psychosocial distress</t>
   </si>
   <si>
@@ -848,13 +803,13 @@
     <t>% HH spending more than 30% of total expenditure on rent</t>
   </si>
   <si>
-    <t>0.0943408235950018</t>
-  </si>
-  <si>
-    <t>0.0859879849718212</t>
-  </si>
-  <si>
-    <t>0.102693662218182</t>
+    <t>0.0933878059519267</t>
+  </si>
+  <si>
+    <t>0.0850507558033352</t>
+  </si>
+  <si>
+    <t>0.101724856100518</t>
   </si>
   <si>
     <t xml:space="preserve">% HH with debt value &gt; 505,000 IQD </t>
@@ -968,7 +923,7 @@
     <t>0.0508292714861747</t>
   </si>
   <si>
-    <t>% HH reporting [reason] as a risk for eviction (analysed for all three years)</t>
+    <t>% HH reporting [reason] as a risk for eviction</t>
   </si>
   <si>
     <t>Lack of funds to pay rental costs</t>
@@ -1005,6 +960,18 @@
   </si>
   <si>
     <t>0.229548310887445</t>
+  </si>
+  <si>
+    <t>Owner Request</t>
+  </si>
+  <si>
+    <t>0.234571794043825</t>
+  </si>
+  <si>
+    <t>0.110462623997151</t>
+  </si>
+  <si>
+    <t>0.3586809640905</t>
   </si>
   <si>
     <t>AAP</t>
@@ -1053,6 +1020,18 @@
 </t>
   </si>
   <si>
+    <t>0.0637427412060089</t>
+  </si>
+  <si>
+    <t>0.042909027192058</t>
+  </si>
+  <si>
+    <t>0.0845764552199597</t>
+  </si>
+  <si>
+    <t>Quantity not enough</t>
+  </si>
+  <si>
     <t>0.0852542361249025</t>
   </si>
   <si>
@@ -1062,15 +1041,30 @@
     <t>0.108332491487483</t>
   </si>
   <si>
-    <t>Quantity not enough</t>
-  </si>
-  <si>
     <t>Delays in delivery of aid</t>
   </si>
   <si>
+    <t>0.0417207831970313</t>
+  </si>
+  <si>
+    <t>0.0299272377137407</t>
+  </si>
+  <si>
+    <t>0.053514328680322</t>
+  </si>
+  <si>
     <t>Other</t>
   </si>
   <si>
+    <t>0.00777183047206496</t>
+  </si>
+  <si>
+    <t>-0.00471305716556476</t>
+  </si>
+  <si>
+    <t>0.0202567181096947</t>
+  </si>
+  <si>
     <t>% of households reporting "health care" as primary information need</t>
   </si>
   <si>
@@ -1146,76 +1140,67 @@
     <t>0.131963284803462</t>
   </si>
   <si>
-    <t>0.234571794043825</t>
-  </si>
-  <si>
-    <t>0.110462623997151</t>
-  </si>
-  <si>
-    <t>0.3586809640905</t>
-  </si>
-  <si>
     <t>% HH reporting [type of difficulty] in accessing health services</t>
   </si>
   <si>
     <t>Cost of services and/or medicine was too high</t>
   </si>
   <si>
-    <t>0.299835667700246</t>
-  </si>
-  <si>
-    <t>0.285214519970443</t>
-  </si>
-  <si>
-    <t>0.31445681543005</t>
+    <t>0.515984688663746</t>
+  </si>
+  <si>
+    <t>0.489260864814829</t>
+  </si>
+  <si>
+    <t>0.542708512512664</t>
   </si>
   <si>
     <t>No medicine available at health facility/pharmacy</t>
   </si>
   <si>
-    <t>0.0836295515130387</t>
-  </si>
-  <si>
-    <t>0.0753184714857409</t>
-  </si>
-  <si>
-    <t>0.0919406315403366</t>
+    <t>0.139419927346377</t>
+  </si>
+  <si>
+    <t>0.124107077497243</t>
+  </si>
+  <si>
+    <t>0.15473277719551</t>
   </si>
   <si>
     <t>Required treatment was not available at health facility</t>
   </si>
   <si>
-    <t>0.0547370280608728</t>
-  </si>
-  <si>
-    <t>0.0470039393094115</t>
-  </si>
-  <si>
-    <t>0.062470116812334</t>
+    <t>0.0885364135692253</t>
+  </si>
+  <si>
+    <t>0.0738455111856383</t>
+  </si>
+  <si>
+    <t>0.103227315952812</t>
   </si>
   <si>
     <t>The treatment center was too far away and/or transportation constraints</t>
   </si>
   <si>
-    <t>0.0372337920186579</t>
-  </si>
-  <si>
-    <t>0.0324228254729766</t>
-  </si>
-  <si>
-    <t>0.0420447585643393</t>
+    <t>0.0537222156238777</t>
+  </si>
+  <si>
+    <t>0.0462720256243094</t>
+  </si>
+  <si>
+    <t>0.0611724056234461</t>
   </si>
   <si>
     <t>Public health clinic was not open</t>
   </si>
   <si>
-    <t>0.0105935865682699</t>
-  </si>
-  <si>
-    <t>0.00751529009417557</t>
-  </si>
-  <si>
-    <t>0.0136718830423642</t>
+    <t>0.0156571003750391</t>
+  </si>
+  <si>
+    <t>0.0110028406900737</t>
+  </si>
+  <si>
+    <t>0.0203113600600046</t>
   </si>
 </sst>
 </file>
@@ -1759,2071 +1744,1981 @@
       <c r="FH1" t="s">
         <v>163</v>
       </c>
-      <c r="FI1" t="s">
-        <v>164</v>
-      </c>
-      <c r="FJ1" t="s">
-        <v>165</v>
-      </c>
-      <c r="FK1" t="s">
-        <v>166</v>
-      </c>
-      <c r="FL1" t="s">
-        <v>167</v>
-      </c>
-      <c r="FM1" t="s">
-        <v>168</v>
-      </c>
-      <c r="FN1" t="s">
-        <v>169</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F2" t="s">
         <v>171</v>
       </c>
-      <c r="D2" t="s">
-        <v>170</v>
-      </c>
-      <c r="E2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F2" t="s">
-        <v>177</v>
-      </c>
       <c r="G2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="H2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="I2" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="J2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="K2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="L2" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="M2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="N2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="O2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="P2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="Q2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="R2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="S2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="T2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="U2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="V2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="W2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="X2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="Y2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="Z2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AA2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="AB2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AC2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AD2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="AE2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AF2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AG2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="AH2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AI2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AJ2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="AK2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AL2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AM2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="AN2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AO2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AP2" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="AQ2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AR2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AS2" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="AT2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AU2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AV2" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="AW2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AX2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AY2" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="AZ2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BA2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BB2" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="BC2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BD2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BE2" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="BF2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BG2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BH2" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="BI2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BJ2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BK2" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="BL2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BM2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BN2" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="BO2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BP2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BQ2" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="BR2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BS2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BT2" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="BU2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BV2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BW2" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="BX2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BY2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BZ2" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="CA2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CB2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CC2" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="CD2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CE2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CF2" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="CG2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CH2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CI2" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="CJ2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CK2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CL2" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="CM2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CN2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CO2" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="CP2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CQ2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CR2" t="s">
-        <v>251</v>
+        <v>223</v>
       </c>
       <c r="CS2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CT2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CU2" t="s">
-        <v>251</v>
+        <v>223</v>
       </c>
       <c r="CV2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CW2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CX2" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="CY2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CZ2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DA2" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="DB2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DC2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DD2" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="DE2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DF2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DG2" t="s">
-        <v>229</v>
+        <v>319</v>
       </c>
       <c r="DH2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DI2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DJ2" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="DK2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DL2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DM2" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="DN2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DO2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DP2" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="DQ2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DR2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DS2" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="DT2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DU2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DV2" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="DW2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DX2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DY2" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="DZ2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EA2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EB2" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="EC2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="ED2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EE2" t="s">
-        <v>330</v>
+        <v>223</v>
       </c>
       <c r="EF2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EG2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EH2" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="EI2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EJ2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EK2" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="EL2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EM2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EN2" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="EO2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EP2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EQ2" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="ER2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="ES2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="ET2" t="s">
-        <v>251</v>
+        <v>324</v>
       </c>
       <c r="EU2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EV2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EW2" t="s">
-        <v>251</v>
+        <v>324</v>
       </c>
       <c r="EX2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EY2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EZ2" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
       <c r="FA2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="FB2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="FC2" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
       <c r="FD2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="FE2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="FF2" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
       <c r="FG2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="FH2" t="s">
-        <v>170</v>
-      </c>
-      <c r="FI2" t="s">
-        <v>335</v>
-      </c>
-      <c r="FJ2" t="s">
-        <v>170</v>
-      </c>
-      <c r="FK2" t="s">
-        <v>170</v>
-      </c>
-      <c r="FL2" t="s">
-        <v>335</v>
-      </c>
-      <c r="FM2" t="s">
-        <v>170</v>
-      </c>
-      <c r="FN2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E3" t="s">
+        <v>164</v>
+      </c>
+      <c r="F3" t="s">
         <v>172</v>
       </c>
-      <c r="D3" t="s">
-        <v>170</v>
-      </c>
-      <c r="E3" t="s">
-        <v>170</v>
-      </c>
-      <c r="F3" t="s">
-        <v>178</v>
-      </c>
       <c r="G3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="H3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="I3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="J3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="K3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="L3" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="M3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="N3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="O3" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="P3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="Q3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="R3" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="S3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="T3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="U3" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="V3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="W3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="X3" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="Y3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="Z3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AA3" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="AB3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AC3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AD3" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="AE3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AF3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AG3" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="AH3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AI3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AJ3" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="AK3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AL3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AM3" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="AN3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AO3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AP3" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="AQ3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AR3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AS3" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="AT3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AU3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AV3" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="AW3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AX3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AY3" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="AZ3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BA3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BB3" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="BC3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BD3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BE3" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="BF3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BG3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BH3" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="BI3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BJ3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BK3" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="BL3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BM3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BN3" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="BO3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BP3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BQ3" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="BR3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BS3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BT3" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="BU3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BV3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BW3" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="BX3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BY3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BZ3" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="CA3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CB3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CC3" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="CD3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CE3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CF3" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="CG3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CH3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CI3" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="CJ3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CK3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CL3" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="CM3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CN3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CO3" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="CP3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CQ3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CR3" t="s">
-        <v>288</v>
+        <v>298</v>
       </c>
       <c r="CS3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CT3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CU3" t="s">
-        <v>288</v>
+        <v>302</v>
       </c>
       <c r="CV3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CW3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CX3" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="CY3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CZ3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DA3" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
       <c r="DB3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DC3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DD3" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
       <c r="DE3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DF3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DG3" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="DH3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DI3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DJ3" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="DK3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DL3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DM3" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="DN3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DO3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DP3" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="DQ3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DR3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DS3" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="DT3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DU3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DV3" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="DW3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DX3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DY3" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="DZ3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EA3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EB3" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
       <c r="EC3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="ED3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EE3" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="EF3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EG3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EH3" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="EI3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EJ3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EK3" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="EL3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EM3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EN3" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="EO3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EP3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EQ3" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="ER3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="ES3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="ET3" t="s">
-        <v>359</v>
+        <v>374</v>
       </c>
       <c r="EU3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EV3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EW3" t="s">
-        <v>313</v>
+        <v>374</v>
       </c>
       <c r="EX3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EY3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EZ3" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="FA3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="FB3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="FC3" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="FD3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="FE3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="FF3" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="FG3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="FH3" t="s">
-        <v>170</v>
-      </c>
-      <c r="FI3" t="s">
-        <v>379</v>
-      </c>
-      <c r="FJ3" t="s">
-        <v>170</v>
-      </c>
-      <c r="FK3" t="s">
-        <v>170</v>
-      </c>
-      <c r="FL3" t="s">
-        <v>379</v>
-      </c>
-      <c r="FM3" t="s">
-        <v>170</v>
-      </c>
-      <c r="FN3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D4" t="s">
+        <v>164</v>
+      </c>
+      <c r="E4" t="s">
+        <v>164</v>
+      </c>
+      <c r="F4" t="s">
         <v>172</v>
       </c>
-      <c r="D4" t="s">
-        <v>170</v>
-      </c>
-      <c r="E4" t="s">
-        <v>170</v>
-      </c>
-      <c r="F4" t="s">
-        <v>178</v>
-      </c>
       <c r="G4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="H4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="I4" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="J4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="K4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="L4" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="M4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="N4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="O4" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="P4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="Q4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="R4" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="S4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="T4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="U4" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="V4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="W4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="X4" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="Y4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="Z4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AA4" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="AB4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AC4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AD4" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="AE4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AF4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AG4" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="AH4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AI4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AJ4" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="AK4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AL4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AM4" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="AN4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AO4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AP4" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="AQ4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AR4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AS4" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="AT4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AU4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AV4" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="AW4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AX4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AY4" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="AZ4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BA4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BB4" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="BC4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BD4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BE4" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="BF4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BG4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BH4" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="BI4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BJ4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BK4" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="BL4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BM4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BN4" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="BO4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BP4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BQ4" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="BR4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BS4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BT4" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="BU4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BV4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BW4" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="BX4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BY4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BZ4" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="CA4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CB4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CC4" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="CD4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CE4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CF4" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="CG4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CH4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CI4" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="CJ4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CK4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CL4" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="CM4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CN4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CO4" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="CP4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CQ4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CR4" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="CS4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CT4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CU4" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="CV4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CW4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CX4" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="CY4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CZ4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DA4" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="DB4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DC4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DD4" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="DE4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DF4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DG4" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="DH4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DI4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DJ4" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="DK4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DL4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DM4" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="DN4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DO4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DP4" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="DQ4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DR4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DS4" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="DT4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DU4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DV4" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="DW4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DX4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DY4" t="s">
+        <v>345</v>
+      </c>
+      <c r="DZ4" t="s">
+        <v>164</v>
+      </c>
+      <c r="EA4" t="s">
+        <v>164</v>
+      </c>
+      <c r="EB4" t="s">
         <v>349</v>
       </c>
-      <c r="DZ4" t="s">
-        <v>170</v>
-      </c>
-      <c r="EA4" t="s">
-        <v>170</v>
-      </c>
-      <c r="EB4" t="s">
-        <v>350</v>
-      </c>
       <c r="EC4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="ED4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EE4" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="EF4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EG4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EH4" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="EI4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EJ4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EK4" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="EL4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EM4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EN4" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="EO4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EP4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EQ4" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="ER4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="ES4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="ET4" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="EU4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EV4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EW4" t="s">
-        <v>313</v>
+        <v>379</v>
       </c>
       <c r="EX4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EY4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EZ4" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="FA4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="FB4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="FC4" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="FD4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="FE4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="FF4" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="FG4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="FH4" t="s">
-        <v>170</v>
-      </c>
-      <c r="FI4" t="s">
-        <v>392</v>
-      </c>
-      <c r="FJ4" t="s">
-        <v>170</v>
-      </c>
-      <c r="FK4" t="s">
-        <v>170</v>
-      </c>
-      <c r="FL4" t="s">
-        <v>396</v>
-      </c>
-      <c r="FM4" t="s">
-        <v>170</v>
-      </c>
-      <c r="FN4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="E5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="G5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="H5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="I5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="J5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="K5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="L5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="M5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="N5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="O5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="P5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="Q5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="R5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="S5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="T5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="U5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="V5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="W5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="X5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="Y5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="Z5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AA5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="AB5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AC5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AD5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="AE5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AF5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AG5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="AH5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AI5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AJ5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="AK5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AL5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AM5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="AN5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AO5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AP5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="AQ5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AR5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AS5" t="s">
-        <v>235</v>
+        <v>167</v>
       </c>
       <c r="AT5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AU5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AV5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="AW5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AX5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AY5" t="s">
-        <v>235</v>
+        <v>167</v>
       </c>
       <c r="AZ5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BA5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BB5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="BC5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BD5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BE5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="BF5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BG5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BH5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="BI5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BJ5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BK5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="BL5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BM5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BN5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="BO5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BP5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BQ5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="BR5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BS5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BT5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="BU5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BV5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BW5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="BX5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BY5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BZ5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="CA5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CB5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CC5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="CD5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CE5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CF5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="CG5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CH5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CI5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="CJ5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CK5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CL5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="CM5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CN5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CO5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="CP5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CQ5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CR5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="CS5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CT5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CU5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="CV5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CW5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CX5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="CY5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="CZ5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DA5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="DB5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DC5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DD5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="DE5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DF5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DG5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="DH5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DI5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DJ5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="DK5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DL5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DM5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="DN5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DO5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DP5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="DQ5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DR5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DS5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="DT5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DU5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DV5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="DW5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DX5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="DY5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="DZ5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EA5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EB5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="EC5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="ED5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EE5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="EF5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EG5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EH5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="EI5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EJ5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EK5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="EL5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EM5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EN5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="EO5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EP5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EQ5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="ER5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="ES5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="ET5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="EU5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EV5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EW5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="EX5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EY5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="EZ5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="FA5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="FB5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="FC5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="FD5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="FE5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="FF5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="FG5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="FH5" t="s">
-        <v>170</v>
-      </c>
-      <c r="FI5" t="s">
-        <v>173</v>
-      </c>
-      <c r="FJ5" t="s">
-        <v>170</v>
-      </c>
-      <c r="FK5" t="s">
-        <v>170</v>
-      </c>
-      <c r="FL5" t="s">
-        <v>173</v>
-      </c>
-      <c r="FM5" t="s">
-        <v>170</v>
-      </c>
-      <c r="FN5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6">
@@ -3834,508 +3729,490 @@
         <v>#N/A</v>
       </c>
       <c r="C6" t="s">
+        <v>168</v>
+      </c>
+      <c r="D6" t="s">
+        <v>169</v>
+      </c>
+      <c r="E6" t="s">
+        <v>170</v>
+      </c>
+      <c r="F6" t="s">
+        <v>173</v>
+      </c>
+      <c r="G6" t="s">
         <v>174</v>
       </c>
-      <c r="D6" t="s">
+      <c r="H6" t="s">
         <v>175</v>
       </c>
-      <c r="E6" t="s">
-        <v>176</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="I6" t="s">
+        <v>177</v>
+      </c>
+      <c r="J6" t="s">
+        <v>178</v>
+      </c>
+      <c r="K6" t="s">
         <v>179</v>
       </c>
-      <c r="G6" t="s">
-        <v>180</v>
-      </c>
-      <c r="H6" t="s">
-        <v>181</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="L6" t="s">
+        <v>182</v>
+      </c>
+      <c r="M6" t="s">
         <v>183</v>
       </c>
-      <c r="J6" t="s">
+      <c r="N6" t="s">
         <v>184</v>
       </c>
-      <c r="K6" t="s">
-        <v>185</v>
-      </c>
-      <c r="L6" t="s">
+      <c r="O6" t="s">
+        <v>187</v>
+      </c>
+      <c r="P6" t="s">
         <v>188</v>
       </c>
-      <c r="M6" t="s">
+      <c r="Q6" t="s">
         <v>189</v>
       </c>
-      <c r="N6" t="s">
-        <v>190</v>
-      </c>
-      <c r="O6" t="s">
+      <c r="R6" t="s">
+        <v>191</v>
+      </c>
+      <c r="S6" t="s">
+        <v>192</v>
+      </c>
+      <c r="T6" t="s">
         <v>193</v>
       </c>
-      <c r="P6" t="s">
-        <v>194</v>
-      </c>
-      <c r="Q6" t="s">
+      <c r="U6" t="s">
         <v>195</v>
       </c>
-      <c r="R6" t="s">
+      <c r="V6" t="s">
+        <v>196</v>
+      </c>
+      <c r="W6" t="s">
         <v>197</v>
       </c>
-      <c r="S6" t="s">
-        <v>198</v>
-      </c>
-      <c r="T6" t="s">
-        <v>199</v>
-      </c>
-      <c r="U6" t="s">
+      <c r="X6" t="s">
+        <v>200</v>
+      </c>
+      <c r="Y6" t="s">
         <v>201</v>
       </c>
-      <c r="V6" t="s">
+      <c r="Z6" t="s">
         <v>202</v>
       </c>
-      <c r="W6" t="s">
-        <v>203</v>
-      </c>
-      <c r="X6" t="s">
+      <c r="AA6" t="s">
+        <v>204</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>205</v>
+      </c>
+      <c r="AC6" t="s">
         <v>206</v>
       </c>
-      <c r="Y6" t="s">
-        <v>207</v>
-      </c>
-      <c r="Z6" t="s">
+      <c r="AD6" t="s">
         <v>208</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AE6" t="s">
+        <v>209</v>
+      </c>
+      <c r="AF6" t="s">
         <v>210</v>
       </c>
-      <c r="AB6" t="s">
-        <v>211</v>
-      </c>
-      <c r="AC6" t="s">
+      <c r="AG6" t="s">
         <v>212</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AH6" t="s">
+        <v>213</v>
+      </c>
+      <c r="AI6" t="s">
         <v>214</v>
       </c>
-      <c r="AE6" t="s">
-        <v>215</v>
-      </c>
-      <c r="AF6" t="s">
+      <c r="AJ6" t="s">
         <v>216</v>
       </c>
-      <c r="AG6" t="s">
+      <c r="AK6" t="s">
+        <v>217</v>
+      </c>
+      <c r="AL6" t="s">
         <v>218</v>
       </c>
-      <c r="AH6" t="s">
-        <v>219</v>
-      </c>
-      <c r="AI6" t="s">
+      <c r="AM6" t="s">
         <v>220</v>
       </c>
-      <c r="AJ6" t="s">
+      <c r="AN6" t="s">
+        <v>221</v>
+      </c>
+      <c r="AO6" t="s">
         <v>222</v>
       </c>
-      <c r="AK6" t="s">
-        <v>223</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>224</v>
-      </c>
-      <c r="AM6" t="s">
+      <c r="AP6" t="s">
+        <v>225</v>
+      </c>
+      <c r="AQ6" t="s">
         <v>226</v>
       </c>
-      <c r="AN6" t="s">
+      <c r="AR6" t="s">
         <v>227</v>
       </c>
-      <c r="AO6" t="s">
-        <v>228</v>
-      </c>
-      <c r="AP6" t="s">
+      <c r="AS6" t="s">
+        <v>229</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>230</v>
+      </c>
+      <c r="AU6" t="s">
         <v>231</v>
       </c>
-      <c r="AQ6" t="s">
-        <v>232</v>
-      </c>
-      <c r="AR6" t="s">
+      <c r="AV6" t="s">
         <v>233</v>
       </c>
-      <c r="AS6" t="s">
-        <v>236</v>
-      </c>
-      <c r="AT6" t="s">
-        <v>237</v>
-      </c>
-      <c r="AU6" t="s">
+      <c r="AW6" t="s">
+        <v>234</v>
+      </c>
+      <c r="AX6" t="s">
+        <v>235</v>
+      </c>
+      <c r="AY6" t="s">
         <v>238</v>
       </c>
-      <c r="AV6" t="s">
+      <c r="AZ6" t="s">
+        <v>239</v>
+      </c>
+      <c r="BA6" t="s">
         <v>240</v>
       </c>
-      <c r="AW6" t="s">
-        <v>241</v>
-      </c>
-      <c r="AX6" t="s">
+      <c r="BB6" t="s">
         <v>242</v>
       </c>
-      <c r="AY6" t="s">
+      <c r="BC6" t="s">
+        <v>243</v>
+      </c>
+      <c r="BD6" t="s">
         <v>244</v>
       </c>
-      <c r="AZ6" t="s">
-        <v>245</v>
-      </c>
-      <c r="BA6" t="s">
+      <c r="BE6" t="s">
         <v>246</v>
       </c>
-      <c r="BB6" t="s">
+      <c r="BF6" t="s">
+        <v>247</v>
+      </c>
+      <c r="BG6" t="s">
         <v>248</v>
       </c>
-      <c r="BC6" t="s">
-        <v>249</v>
-      </c>
-      <c r="BD6" t="s">
+      <c r="BH6" t="s">
         <v>250</v>
       </c>
-      <c r="BE6" t="s">
-        <v>253</v>
-      </c>
-      <c r="BF6" t="s">
+      <c r="BI6" t="s">
+        <v>251</v>
+      </c>
+      <c r="BJ6" t="s">
+        <v>252</v>
+      </c>
+      <c r="BK6" t="s">
         <v>254</v>
       </c>
-      <c r="BG6" t="s">
+      <c r="BL6" t="s">
         <v>255</v>
       </c>
-      <c r="BH6" t="s">
-        <v>257</v>
-      </c>
-      <c r="BI6" t="s">
+      <c r="BM6" t="s">
+        <v>256</v>
+      </c>
+      <c r="BN6" t="s">
         <v>258</v>
       </c>
-      <c r="BJ6" t="s">
+      <c r="BO6" t="s">
         <v>259</v>
       </c>
-      <c r="BK6" t="s">
-        <v>261</v>
-      </c>
-      <c r="BL6" t="s">
+      <c r="BP6" t="s">
+        <v>260</v>
+      </c>
+      <c r="BQ6" t="s">
         <v>262</v>
       </c>
-      <c r="BM6" t="s">
+      <c r="BR6" t="s">
         <v>263</v>
       </c>
-      <c r="BN6" t="s">
-        <v>265</v>
-      </c>
-      <c r="BO6" t="s">
+      <c r="BS6" t="s">
+        <v>264</v>
+      </c>
+      <c r="BT6" t="s">
         <v>266</v>
       </c>
-      <c r="BP6" t="s">
+      <c r="BU6" t="s">
         <v>267</v>
       </c>
-      <c r="BQ6" t="s">
-        <v>269</v>
-      </c>
-      <c r="BR6" t="s">
+      <c r="BV6" t="s">
+        <v>268</v>
+      </c>
+      <c r="BW6" t="s">
         <v>270</v>
       </c>
-      <c r="BS6" t="s">
+      <c r="BX6" t="s">
         <v>271</v>
       </c>
-      <c r="BT6" t="s">
-        <v>273</v>
-      </c>
-      <c r="BU6" t="s">
-        <v>274</v>
-      </c>
-      <c r="BV6" t="s">
+      <c r="BY6" t="s">
+        <v>272</v>
+      </c>
+      <c r="BZ6" t="s">
         <v>275</v>
       </c>
-      <c r="BW6" t="s">
+      <c r="CA6" t="s">
+        <v>276</v>
+      </c>
+      <c r="CB6" t="s">
         <v>277</v>
       </c>
-      <c r="BX6" t="s">
-        <v>278</v>
-      </c>
-      <c r="BY6" t="s">
+      <c r="CC6" t="s">
         <v>279</v>
       </c>
-      <c r="BZ6" t="s">
+      <c r="CD6" t="s">
+        <v>280</v>
+      </c>
+      <c r="CE6" t="s">
         <v>281</v>
       </c>
-      <c r="CA6" t="s">
-        <v>282</v>
-      </c>
-      <c r="CB6" t="s">
+      <c r="CF6" t="s">
         <v>283</v>
       </c>
-      <c r="CC6" t="s">
+      <c r="CG6" t="s">
+        <v>284</v>
+      </c>
+      <c r="CH6" t="s">
         <v>285</v>
       </c>
-      <c r="CD6" t="s">
-        <v>286</v>
-      </c>
-      <c r="CE6" t="s">
+      <c r="CI6" t="s">
         <v>287</v>
       </c>
-      <c r="CF6" t="s">
-        <v>290</v>
-      </c>
-      <c r="CG6" t="s">
+      <c r="CJ6" t="s">
+        <v>288</v>
+      </c>
+      <c r="CK6" t="s">
+        <v>289</v>
+      </c>
+      <c r="CL6" t="s">
         <v>291</v>
       </c>
-      <c r="CH6" t="s">
+      <c r="CM6" t="s">
         <v>292</v>
       </c>
-      <c r="CI6" t="s">
-        <v>294</v>
-      </c>
-      <c r="CJ6" t="s">
+      <c r="CN6" t="s">
+        <v>293</v>
+      </c>
+      <c r="CO6" t="s">
         <v>295</v>
       </c>
-      <c r="CK6" t="s">
+      <c r="CP6" t="s">
         <v>296</v>
       </c>
-      <c r="CL6" t="s">
-        <v>298</v>
-      </c>
-      <c r="CM6" t="s">
+      <c r="CQ6" t="s">
+        <v>297</v>
+      </c>
+      <c r="CR6" t="s">
         <v>299</v>
       </c>
-      <c r="CN6" t="s">
+      <c r="CS6" t="s">
         <v>300</v>
       </c>
-      <c r="CO6" t="s">
-        <v>302</v>
-      </c>
-      <c r="CP6" t="s">
-        <v>303</v>
-      </c>
-      <c r="CQ6" t="s">
+      <c r="CT6" t="s">
+        <v>301</v>
+      </c>
+      <c r="CU6" t="s">
         <v>304</v>
       </c>
-      <c r="CR6" t="s">
+      <c r="CV6" t="s">
+        <v>305</v>
+      </c>
+      <c r="CW6" t="s">
         <v>306</v>
       </c>
-      <c r="CS6" t="s">
-        <v>307</v>
-      </c>
-      <c r="CT6" t="s">
+      <c r="CX6" t="s">
         <v>308</v>
       </c>
-      <c r="CU6" t="s">
+      <c r="CY6" t="s">
+        <v>309</v>
+      </c>
+      <c r="CZ6" t="s">
         <v>310</v>
       </c>
-      <c r="CV6" t="s">
-        <v>311</v>
-      </c>
-      <c r="CW6" t="s">
+      <c r="DA6" t="s">
         <v>312</v>
       </c>
-      <c r="CX6" t="s">
+      <c r="DB6" t="s">
+        <v>313</v>
+      </c>
+      <c r="DC6" t="s">
         <v>314</v>
       </c>
-      <c r="CY6" t="s">
-        <v>315</v>
-      </c>
-      <c r="CZ6" t="s">
+      <c r="DD6" t="s">
         <v>316</v>
       </c>
-      <c r="DA6" t="s">
-        <v>319</v>
-      </c>
-      <c r="DB6" t="s">
-        <v>320</v>
-      </c>
-      <c r="DC6" t="s">
+      <c r="DE6" t="s">
+        <v>317</v>
+      </c>
+      <c r="DF6" t="s">
+        <v>318</v>
+      </c>
+      <c r="DG6" t="s">
         <v>321</v>
       </c>
-      <c r="DD6" t="s">
+      <c r="DH6" t="s">
+        <v>322</v>
+      </c>
+      <c r="DI6" t="s">
         <v>323</v>
       </c>
-      <c r="DE6" t="s">
-        <v>324</v>
-      </c>
-      <c r="DF6" t="s">
+      <c r="DJ6" t="s">
         <v>325</v>
       </c>
-      <c r="DG6" t="s">
+      <c r="DK6" t="s">
+        <v>326</v>
+      </c>
+      <c r="DL6" t="s">
         <v>327</v>
       </c>
-      <c r="DH6" t="s">
-        <v>328</v>
-      </c>
-      <c r="DI6" t="s">
+      <c r="DM6" t="s">
         <v>329</v>
       </c>
-      <c r="DJ6" t="s">
-        <v>332</v>
-      </c>
-      <c r="DK6" t="s">
-        <v>333</v>
-      </c>
-      <c r="DL6" t="s">
+      <c r="DN6" t="s">
+        <v>330</v>
+      </c>
+      <c r="DO6" t="s">
+        <v>331</v>
+      </c>
+      <c r="DP6" t="s">
         <v>334</v>
       </c>
-      <c r="DM6" t="s">
+      <c r="DQ6" t="s">
+        <v>335</v>
+      </c>
+      <c r="DR6" t="s">
         <v>336</v>
       </c>
-      <c r="DN6" t="s">
-        <v>337</v>
-      </c>
-      <c r="DO6" t="s">
+      <c r="DS6" t="s">
         <v>338</v>
       </c>
-      <c r="DP6" t="s">
+      <c r="DT6" t="s">
+        <v>339</v>
+      </c>
+      <c r="DU6" t="s">
         <v>340</v>
       </c>
-      <c r="DQ6" t="s">
-        <v>341</v>
-      </c>
-      <c r="DR6" t="s">
+      <c r="DV6" t="s">
         <v>342</v>
       </c>
-      <c r="DS6" t="s">
-        <v>345</v>
-      </c>
-      <c r="DT6" t="s">
+      <c r="DW6" t="s">
+        <v>343</v>
+      </c>
+      <c r="DX6" t="s">
+        <v>344</v>
+      </c>
+      <c r="DY6" t="s">
         <v>346</v>
       </c>
-      <c r="DU6" t="s">
+      <c r="DZ6" t="s">
         <v>347</v>
       </c>
-      <c r="DV6" t="s">
-        <v>345</v>
-      </c>
-      <c r="DW6" t="s">
-        <v>346</v>
-      </c>
-      <c r="DX6" t="s">
-        <v>347</v>
-      </c>
-      <c r="DY6" t="s">
-        <v>345</v>
-      </c>
-      <c r="DZ6" t="s">
-        <v>346</v>
-      </c>
       <c r="EA6" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="EB6" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="EC6" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="ED6" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
       <c r="EE6" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="EF6" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="EG6" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="EH6" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="EI6" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="EJ6" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="EK6" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="EL6" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="EM6" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="EN6" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="EO6" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="EP6" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="EQ6" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="ER6" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="ES6" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="ET6" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="EU6" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="EV6" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="EW6" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="EX6" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="EY6" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="EZ6" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="FA6" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="FB6" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="FC6" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="FD6" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="FE6" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="FF6" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="FG6" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="FH6" t="s">
-        <v>391</v>
-      </c>
-      <c r="FI6" t="s">
-        <v>393</v>
-      </c>
-      <c r="FJ6" t="s">
         <v>394</v>
-      </c>
-      <c r="FK6" t="s">
-        <v>395</v>
-      </c>
-      <c r="FL6" t="s">
-        <v>397</v>
-      </c>
-      <c r="FM6" t="s">
-        <v>398</v>
-      </c>
-      <c r="FN6" t="s">
-        <v>399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>